<commit_message>
circuit + truth table so far
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfinegan/Documents/Teaching/CurrentCourses/CMSC301/Project/Checkpoint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolozgvelesiani/Desktop/Semester_6/CMSC_301/Project_Assembler/Checkpoint_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F042486-E1D1-9C4D-8F09-9A031C0EC670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F78F75-9F71-434A-B76E-F747401A03E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1780" windowWidth="31360" windowHeight="17440" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
+    <workbookView xWindow="580" yWindow="5620" windowWidth="28800" windowHeight="17440" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>instr</t>
   </si>
@@ -131,22 +131,31 @@
     <t>syscall</t>
   </si>
   <si>
-    <t>31:26</t>
-  </si>
-  <si>
-    <t>25:21</t>
-  </si>
-  <si>
-    <t>20:16</t>
-  </si>
-  <si>
-    <t>15:11</t>
-  </si>
-  <si>
-    <t>10:6</t>
-  </si>
-  <si>
-    <t>5:0</t>
+    <t>31:26(Op code)</t>
+  </si>
+  <si>
+    <t>25:21(rs)</t>
+  </si>
+  <si>
+    <t>20:16(rt)</t>
+  </si>
+  <si>
+    <t>15:11(rd)</t>
+  </si>
+  <si>
+    <t>10:6(shift)</t>
+  </si>
+  <si>
+    <t>5:0(func)</t>
+  </si>
+  <si>
+    <t>shamt</t>
+  </si>
+  <si>
+    <t>——Address——</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -157,7 +166,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +179,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -187,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -204,11 +220,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -216,17 +292,56 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,20 +676,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="8" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="3" customWidth="1"/>
+    <col min="3" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="10.83203125" style="8"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +713,7 @@
       <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -615,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -637,7 +754,7 @@
       <c r="G2">
         <v>100000</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I2" t="s">
@@ -656,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -678,7 +795,7 @@
       <c r="G3" s="5">
         <v>100010</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I3" t="s">
@@ -697,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -710,12 +827,12 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="12" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I4" t="s">
@@ -734,207 +851,750 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5">
+        <v>11000</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5">
+        <v>11010</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5">
+        <v>10010</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="5">
+        <v>10</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>101010</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="B12" s="21">
+        <v>100011</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="20">
+        <v>1</v>
+      </c>
+      <c r="L12" s="20">
+        <v>1</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0</v>
+      </c>
+      <c r="N12" s="26"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="B13" s="27">
+        <v>101011</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="32">
+        <v>0</v>
+      </c>
+      <c r="L13" s="32">
+        <v>1</v>
+      </c>
+      <c r="M13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="B14" s="5">
+        <v>100</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="32">
+        <v>0</v>
+      </c>
+      <c r="L14" s="32">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="B15" s="5">
+        <v>101</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="32">
+        <v>0</v>
+      </c>
+      <c r="L15" s="32">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="B16" s="5">
+        <v>10</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="32">
+        <v>0</v>
+      </c>
+      <c r="L16" s="32">
+        <v>0</v>
+      </c>
+      <c r="M16" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="B17" s="5">
+        <v>11</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="32">
+        <v>1</v>
+      </c>
+      <c r="L17" s="32">
+        <v>0</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="32">
+        <v>0</v>
+      </c>
+      <c r="L18" s="32">
+        <v>0</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1001</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="32">
+        <v>1</v>
+      </c>
+      <c r="L19" s="32">
+        <v>0</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1100</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="32">
+        <v>0</v>
+      </c>
+      <c r="L20" s="32">
+        <v>0</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+    </row>
+    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+    </row>
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+    </row>
+    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="G30" s="5"/>
     </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
     <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="J17" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
circuits +  truth table
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolozgvelesiani/Desktop/Semester_6/CMSC_301/Project_Assembler/Checkpoint_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F78F75-9F71-434A-B76E-F747401A03E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A7D62-F1A6-5744-866D-54BD71DA1F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="5620" windowWidth="28800" windowHeight="17440" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
@@ -679,7 +679,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edit CPU main and excel file
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolozgvelesiani/Desktop/Semester_6/CMSC_301/Project_Assembler/Checkpoint_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A7D62-F1A6-5744-866D-54BD71DA1F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31A8249-659F-44FF-8B1B-B4E89D2AE7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="5620" windowWidth="28800" windowHeight="17440" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -295,16 +295,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -313,38 +305,32 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -360,7 +346,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -676,22 +662,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="3" customWidth="1"/>
-    <col min="3" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="8" width="10.83203125" style="8"/>
+    <col min="3" max="7" width="10.796875" style="3"/>
+    <col min="8" max="8" width="10.796875" style="8"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -773,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -814,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -827,11 +813,11 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
@@ -851,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -886,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -921,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -953,7 +939,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -985,7 +971,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1007,10 +993,10 @@
       <c r="H9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="I9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K9">
@@ -1023,7 +1009,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1045,7 +1031,7 @@
       <c r="H10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J10" t="s">
@@ -1061,7 +1047,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1083,10 +1069,10 @@
       <c r="H11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="12" t="s">
+      <c r="I11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K11">
@@ -1099,218 +1085,221 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="17">
         <v>100011</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="30" t="s">
+      <c r="C12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="20">
-        <v>1</v>
-      </c>
-      <c r="L12" s="20">
-        <v>1</v>
-      </c>
-      <c r="M12" s="25">
-        <v>0</v>
-      </c>
-      <c r="N12" s="26"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="16">
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <v>1</v>
+      </c>
+      <c r="M12" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="5">
         <v>101011</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="33" t="s">
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="32">
-        <v>0</v>
-      </c>
-      <c r="L13" s="32">
-        <v>1</v>
-      </c>
-      <c r="M13" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="5">
         <v>100</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="33" t="s">
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="32">
-        <v>0</v>
-      </c>
-      <c r="L14" s="32">
+      <c r="I14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>1</v>
       </c>
       <c r="M14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="5">
         <v>101</v>
       </c>
-      <c r="C15" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="36" t="s">
+      <c r="C15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="32">
-        <v>0</v>
-      </c>
-      <c r="L15" s="32">
+      <c r="I15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>1</v>
       </c>
       <c r="M15" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="5">
         <v>10</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="C16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="32">
-        <v>0</v>
-      </c>
-      <c r="L16" s="32">
-        <v>0</v>
-      </c>
-      <c r="M16" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5">
         <v>11</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="C17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="12" t="s">
+      <c r="I17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="32">
-        <v>1</v>
-      </c>
-      <c r="L17" s="32">
-        <v>0</v>
-      </c>
-      <c r="M17" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1326,23 +1315,23 @@
       <c r="H18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="32">
-        <v>0</v>
-      </c>
-      <c r="L18" s="32">
-        <v>0</v>
-      </c>
-      <c r="M18" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1361,23 +1350,23 @@
       <c r="H19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="32">
-        <v>1</v>
-      </c>
-      <c r="L19" s="32">
-        <v>0</v>
-      </c>
-      <c r="M19" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1390,206 +1379,158 @@
       <c r="H20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="32">
-        <v>0</v>
-      </c>
-      <c r="L20" s="32">
-        <v>0</v>
-      </c>
-      <c r="M20" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="14"/>
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="14"/>
+    </row>
+    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="14"/>
+    </row>
+    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="14"/>
+    </row>
+    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="9"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="14"/>
+    </row>
+    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="14"/>
+    </row>
+    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="14"/>
+    </row>
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="14"/>
+    </row>
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="9"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="G39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added challenge instructions to the excel file
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31A8249-659F-44FF-8B1B-B4E89D2AE7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D97AE9-1E07-46F2-AEFF-FAB18F360F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="50">
   <si>
     <t>instr</t>
   </si>
@@ -156,6 +156,36 @@
   </si>
   <si>
     <t>31</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>andi</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>ori</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>xori</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>lui</t>
+  </si>
+  <si>
+    <t>clo</t>
+  </si>
+  <si>
+    <t>clz</t>
   </si>
 </sst>
 </file>
@@ -203,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -218,26 +248,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -284,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -294,18 +304,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -313,7 +316,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -322,12 +325,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -662,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -813,11 +820,11 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1086,48 +1093,49 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="17">
-        <v>100011</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="16">
-        <v>1</v>
-      </c>
-      <c r="L12" s="16">
-        <v>1</v>
-      </c>
-      <c r="M12" s="20">
-        <v>0</v>
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5">
+        <v>11000</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1001</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B13" s="5">
-        <v>101011</v>
+        <v>1100</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
@@ -1135,36 +1143,36 @@
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="M13" s="4">
-        <v>0</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
@@ -1172,136 +1180,146 @@
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5">
+        <v>11001</v>
+      </c>
       <c r="H14" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>14</v>
+      <c r="J14" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="4">
-        <v>1</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B15" s="5">
-        <v>101</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="23" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15" s="4">
-        <v>1</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B16" s="5">
-        <v>10</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="5">
+        <v>11010</v>
+      </c>
       <c r="H16" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" s="22" t="s">
-        <v>14</v>
+      <c r="M16" s="4">
+        <v>1011</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B17" s="5">
-        <v>11</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
+        <v>111110</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1011</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
@@ -1309,233 +1327,470 @@
       <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="G18" s="5">
-        <v>1000</v>
+        <v>11011</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" s="22" t="s">
-        <v>14</v>
+      <c r="M18" s="4">
+        <v>1100</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1001</v>
-      </c>
+        <v>111111</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5">
+        <v>11100</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="5">
+        <v>100001</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="5">
+        <v>11100</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="5">
+        <v>100000</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10">
+        <v>100011</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9">
+        <v>1</v>
+      </c>
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5">
+        <v>101011</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>100</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5">
+        <v>101</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5">
+        <v>10</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5">
+        <v>11</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="5">
+        <v>1001</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
         <v>1100</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="5"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="H30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="E13:G13"/>
     <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E25:G25"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="J17" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change ALU code for lui to 0b1111; Add lui, clo, clz in the circuit
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D97AE9-1E07-46F2-AEFF-FAB18F360F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB990B-3CD0-416C-9AD5-F1D72983DE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -334,7 +334,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -671,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1117,7 +1116,7 @@
       <c r="I12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K12">
@@ -1154,7 +1153,7 @@
       <c r="I13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K13">
@@ -1192,7 +1191,7 @@
       <c r="I14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K14">
@@ -1229,7 +1228,7 @@
       <c r="I15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K15">
@@ -1267,7 +1266,7 @@
       <c r="I16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K16">
@@ -1304,7 +1303,7 @@
       <c r="I17" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K17">
@@ -1342,7 +1341,7 @@
       <c r="I18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K18">
@@ -1376,7 +1375,7 @@
       <c r="I19" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K19">
@@ -1386,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="4">
-        <v>1</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1778,6 +1777,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="C26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="E13:G13"/>
@@ -1785,10 +1788,6 @@
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix bug ALU code giving a non-zero value when it I-type instruction
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C044C11-6AC4-4DD1-98BB-1DDFA8C12FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E362A-CFBC-4619-BB58-425E959AD091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="51">
   <si>
     <t>instr</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>clz</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -312,6 +315,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,12 +334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -818,11 +821,11 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1141,11 +1144,11 @@
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1216,11 +1219,11 @@
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
@@ -1291,11 +1294,11 @@
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
@@ -1363,11 +1366,11 @@
       <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="8" t="s">
         <v>14</v>
       </c>
@@ -1472,11 +1475,11 @@
       <c r="D22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="12" t="s">
         <v>8</v>
       </c>
@@ -1509,11 +1512,11 @@
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="8" t="s">
         <v>8</v>
       </c>
@@ -1546,11 +1549,11 @@
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="8" t="s">
         <v>8</v>
       </c>
@@ -1583,11 +1586,11 @@
       <c r="D25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="8" t="s">
         <v>8</v>
       </c>
@@ -1611,16 +1614,16 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
-        <v>10</v>
-      </c>
-      <c r="C26" s="20" t="s">
+      <c r="B26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1647,13 +1650,13 @@
       <c r="B27" s="5">
         <v>11</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
       <c r="H27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1776,17 +1779,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="C26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix PC counter and j bug
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E362A-CFBC-4619-BB58-425E959AD091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E20B782-2D91-44D6-BAA3-D710FB4048E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
   <si>
     <t>instr</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>clz</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -315,12 +312,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,6 +325,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -821,11 +818,11 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1144,11 +1141,11 @@
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1219,11 +1216,11 @@
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
@@ -1294,11 +1291,11 @@
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
@@ -1366,11 +1363,11 @@
       <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="8" t="s">
         <v>14</v>
       </c>
@@ -1475,11 +1472,11 @@
       <c r="D22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="12" t="s">
         <v>8</v>
       </c>
@@ -1512,11 +1509,11 @@
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
       <c r="H23" s="8" t="s">
         <v>8</v>
       </c>
@@ -1549,11 +1546,11 @@
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="21"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="8" t="s">
         <v>8</v>
       </c>
@@ -1586,11 +1583,11 @@
       <c r="D25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="8" t="s">
         <v>8</v>
       </c>
@@ -1614,16 +1611,16 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="5">
+        <v>10</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
       <c r="H26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1650,13 +1647,13 @@
       <c r="B27" s="5">
         <v>11</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
       <c r="H27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1779,17 +1776,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add ALU code fix for gate operations
</commit_message>
<xml_diff>
--- a/Checkpoint_2/truth_table_starter.xlsx
+++ b/Checkpoint_2/truth_table_starter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\유상현\data\2025 Junior Spring\CMSC301 Computer Organization\Project\Assembly-Assembler\Checkpoint_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolozgvelesiani/Desktop/Semester_6/CMSC_301/Project_Assembler/Checkpoint_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E20B782-2D91-44D6-BAA3-D710FB4048E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C1B24E-B998-1549-A156-0E1355A70746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{3CC5E16A-84AD-254C-A80D-CBE2F9156C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -312,6 +312,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -327,15 +333,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -669,20 +669,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B12971-82CC-C243-B603-E6DE4D0DBF7D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="122" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="3" customWidth="1"/>
-    <col min="3" max="7" width="10.796875" style="3"/>
-    <col min="8" max="8" width="10.796875" style="8"/>
+    <col min="3" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="10.83203125" style="8"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -818,11 +818,11 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -877,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -912,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -944,7 +944,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -976,7 +976,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="5">
-        <v>11000</v>
+        <v>100100</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>8</v>
@@ -1128,7 +1128,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1141,11 +1141,11 @@
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="5">
-        <v>11001</v>
+        <v>100101</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>8</v>
@@ -1203,12 +1203,12 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="5">
-        <v>1110</v>
+        <v>1101</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -1216,11 +1216,11 @@
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="5">
-        <v>11010</v>
+        <v>100110</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>8</v>
@@ -1278,12 +1278,12 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="5">
-        <v>111110</v>
+        <v>1110</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1291,11 +1291,11 @@
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="5">
-        <v>11011</v>
+        <v>100111</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>8</v>
@@ -1353,7 +1353,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1363,11 +1363,11 @@
       <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="8" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
@@ -1472,11 +1472,11 @@
       <c r="D22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="12" t="s">
         <v>8</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1509,11 +1509,11 @@
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="8" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1546,11 +1546,11 @@
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="8" t="s">
         <v>8</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1583,11 +1583,11 @@
       <c r="D25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="8" t="s">
         <v>8</v>
       </c>
@@ -1607,20 +1607,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="5">
         <v>10</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1640,20 +1640,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="5">
         <v>11</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
       <c r="H27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="5">
-        <v>1100</v>
+        <v>1001</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>14</v>
@@ -1776,17 +1776,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="C26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>